<commit_message>
corregida matriz de riesgo
</commit_message>
<xml_diff>
--- a/Fase 1/Evidencias Proyecto/Matriz de riesgo.xlsx
+++ b/Fase 1/Evidencias Proyecto/Matriz de riesgo.xlsx
@@ -1,13 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\duoc\Portafolio\Enmistiempos\Fase 1\Evidencias Proyecto\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA85B0D6-24CE-473B-8E5E-C6C6112E8B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Matriz 2.0" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Mapa de Calor" sheetId="2" r:id="rId5"/>
+    <sheet name="Matriz 2.0" sheetId="1" r:id="rId1"/>
+    <sheet name="Mapa de Calor" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -251,43 +273,54 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -313,9 +346,27 @@
         <bgColor rgb="FF38761D"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -329,137 +380,123 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB7B7B7"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB7B7B7"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB7B7B7"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB7B7B7"/>
-      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF990000"/>
+          <bgColor rgb="FF990000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE69138"/>
+          <bgColor rgb="FFE69138"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF38761D"/>
           <bgColor rgb="FF38761D"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE69138"/>
-          <bgColor rgb="FFE69138"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF990000"/>
-          <bgColor rgb="FF990000"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -649,26 +686,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="2.88"/>
-    <col customWidth="1" min="2" max="4" width="31.38"/>
-    <col customWidth="1" min="5" max="7" width="11.13"/>
-    <col customWidth="1" min="8" max="8" width="50.13"/>
+    <col min="1" max="1" width="2.90625" customWidth="1"/>
+    <col min="2" max="4" width="31.36328125" customWidth="1"/>
+    <col min="5" max="7" width="11.08984375" customWidth="1"/>
+    <col min="8" max="8" width="50.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -697,9 +739,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>9</v>
@@ -710,14 +752,14 @@
       <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="5">
-        <f t="shared" ref="G2:G15" si="1">IF(AND(E2="Alta",F2="Alto"),$K$3*$K$3,IF(AND(E2="Alta",F2="Medio"),$K$3*$K$4,IF(AND(E2="Alta",F2="Bajo"),$K$3*$K$5,IF(AND(E2="Media",F2="Alto"),$K$4*$K$3,IF(AND(E2="Media",F2="Medio"),$K$4*$K$4,IF(AND(E2="Media",F2="Bajo"),$K$4*$K$5,IF(AND(E2="Baja",F2="Alto"),$K$5*$K$3,IF(AND(E2="Baja",F2="Medio"),$K$5*$K$4,IF(AND(E2="Baja",F2="Bajo"),$K$5*$K$5,0)))))))))</f>
+      <c r="G2" s="17">
+        <f t="shared" ref="G2:G15" si="0">IF(AND(E2="Alta",F2="Alto"),$K$3*$K$3,IF(AND(E2="Alta",F2="Medio"),$K$3*$K$4,IF(AND(E2="Alta",F2="Bajo"),$K$3*$K$5,IF(AND(E2="Media",F2="Alto"),$K$4*$K$3,IF(AND(E2="Media",F2="Medio"),$K$4*$K$4,IF(AND(E2="Media",F2="Bajo"),$K$4*$K$5,IF(AND(E2="Baja",F2="Alto"),$K$5*$K$3,IF(AND(E2="Baja",F2="Medio"),$K$5*$K$4,IF(AND(E2="Baja",F2="Bajo"),$K$5*$K$5,0)))))))))</f>
         <v>9</v>
       </c>
       <c r="H2" s="4" t="s">
@@ -727,9 +769,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>16</v>
@@ -740,14 +782,14 @@
       <c r="D3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="5">
-        <f t="shared" si="1"/>
+      <c r="G3" s="17">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="H3" s="4" t="s">
@@ -757,12 +799,12 @@
         <v>12</v>
       </c>
       <c r="K3" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>20</v>
@@ -773,14 +815,14 @@
       <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="5">
-        <f t="shared" si="1"/>
+      <c r="G4" s="17">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="H4" s="4" t="s">
@@ -790,12 +832,12 @@
         <v>24</v>
       </c>
       <c r="K4" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>25</v>
@@ -806,14 +848,14 @@
       <c r="D5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="5">
-        <f t="shared" si="1"/>
+      <c r="G5" s="17">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -823,12 +865,12 @@
         <v>28</v>
       </c>
       <c r="K5" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>31</v>
@@ -839,23 +881,23 @@
       <c r="D6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="5">
-        <f t="shared" si="1"/>
+      <c r="G6" s="17">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>36</v>
@@ -866,23 +908,23 @@
       <c r="D7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="5">
-        <f t="shared" si="1"/>
+      <c r="G7" s="17">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>40</v>
@@ -893,23 +935,23 @@
       <c r="D8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="5">
-        <f t="shared" si="1"/>
+      <c r="G8" s="17">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>44</v>
@@ -920,23 +962,23 @@
       <c r="D9" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="5">
-        <f t="shared" si="1"/>
+      <c r="G9" s="17">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>48</v>
@@ -947,23 +989,23 @@
       <c r="D10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="5">
-        <f t="shared" si="1"/>
+      <c r="G10" s="17">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>52</v>
@@ -974,23 +1016,23 @@
       <c r="D11" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="5">
-        <f t="shared" si="1"/>
+      <c r="G11" s="17">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>56</v>
@@ -1001,23 +1043,23 @@
       <c r="D12" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="5">
-        <f t="shared" si="1"/>
+      <c r="G12" s="17">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>60</v>
@@ -1028,23 +1070,23 @@
       <c r="D13" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="5">
-        <f t="shared" si="1"/>
+      <c r="G13" s="17">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>64</v>
@@ -1055,23 +1097,23 @@
       <c r="D14" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="5">
-        <f t="shared" si="1"/>
+      <c r="G14" s="17">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>68</v>
@@ -1082,484 +1124,483 @@
       <c r="D15" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G15" s="5">
-        <f t="shared" si="1"/>
+      <c r="G15" s="17">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16">
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-    </row>
-    <row r="18">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-    </row>
-    <row r="21">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-    </row>
-    <row r="22">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-    </row>
-    <row r="23">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-    </row>
-    <row r="24">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-    </row>
-    <row r="25">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-    </row>
-    <row r="26">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-    </row>
-    <row r="27">
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-    </row>
-    <row r="28">
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-    </row>
-    <row r="29">
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-    </row>
-    <row r="30">
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-    </row>
-    <row r="31">
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-    </row>
-    <row r="32">
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-    </row>
-    <row r="33">
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-    </row>
-    <row r="34">
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-    </row>
-    <row r="35">
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-    </row>
-    <row r="36">
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-    </row>
-    <row r="37">
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-    </row>
-    <row r="38">
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-    </row>
-    <row r="39">
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-    </row>
-    <row r="40">
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-    </row>
-    <row r="41">
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-    </row>
-    <row r="42">
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-    </row>
-    <row r="43">
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-    </row>
-    <row r="44">
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+    </row>
+    <row r="38" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G15">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThanOrEqual">
       <formula>2</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G15">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>6</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G15">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThanOrEqual">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A2:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="11.5"/>
-    <col customWidth="1" min="2" max="2" width="63.88"/>
-    <col customWidth="1" min="3" max="3" width="11.5"/>
+    <col min="1" max="1" width="2.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.81640625" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="7" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D2" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="10" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E3" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F3" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G3" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="B3" s="10" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D4" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="14">
-        <v>5.0</v>
-      </c>
-      <c r="F3" s="12" t="s">
+      <c r="E4" s="8">
+        <v>5</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="9">
-        <v>3.0</v>
-      </c>
-      <c r="B4" s="10" t="s">
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D5" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="14" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="12">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="G5" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G6" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="9">
-        <v>5.0</v>
-      </c>
-      <c r="B6" s="10" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>5</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="B7" s="10" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>6</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="9">
-        <v>7.0</v>
-      </c>
-      <c r="B8" s="10" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>7</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="9">
-        <v>8.0</v>
-      </c>
-      <c r="B9" s="10" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="9">
-        <v>9.0</v>
-      </c>
-      <c r="B10" s="10" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
+        <v>9</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="9">
-        <v>10.0</v>
-      </c>
-      <c r="B11" s="10" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
+        <v>10</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="9">
-        <v>11.0</v>
-      </c>
-      <c r="B12" s="10" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
+        <v>11</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="9">
-        <v>12.0</v>
-      </c>
-      <c r="B13" s="10" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
+        <v>12</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="9">
-        <v>13.0</v>
-      </c>
-      <c r="B14" s="10" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
+        <v>13</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="9">
-        <v>14.0</v>
-      </c>
-      <c r="B15" s="10" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="10">
+        <v>14</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>68</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
agregada justificacion de arquitectura | cambio a jpg de diagramas de paquetes y componentes | actualizacion de matriz de riesgo
</commit_message>
<xml_diff>
--- a/Fase 1/Evidencias Proyecto/Matriz de riesgo.xlsx
+++ b/Fase 1/Evidencias Proyecto/Matriz de riesgo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\duoc\Portafolio\Enmistiempos\Fase 1\Evidencias Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA85B0D6-24CE-473B-8E5E-C6C6112E8B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B33658C-AEF1-4580-8AB4-66944377761D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>Severidad</t>
   </si>
   <si>
-    <t>Plan de acción</t>
-  </si>
-  <si>
     <t>Severidad = Probabilidad * Impacto</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>Fallos en la ejecución de la app en ciertos dispositivos</t>
   </si>
   <si>
-    <t>Probar en distintos dispositivos y versiones de Android desde el inicio del desarrollo.</t>
-  </si>
-  <si>
     <t>Errores en la integración de APIs externas</t>
   </si>
   <si>
@@ -268,6 +262,12 @@
   </si>
   <si>
     <t>4 - 9</t>
+  </si>
+  <si>
+    <t>Plan de mitigación</t>
+  </si>
+  <si>
+    <t>Probar en distintos dispositivos y versiones de Android desde el inicio del desarrollo. Definir desde el inicio la versión Android mínima para el funcionamiento de la App.</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -453,6 +453,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,8 +707,10 @@
   <cols>
     <col min="1" max="1" width="2.90625" customWidth="1"/>
     <col min="2" max="4" width="31.36328125" customWidth="1"/>
-    <col min="5" max="7" width="11.08984375" customWidth="1"/>
+    <col min="5" max="7" width="12.6328125" customWidth="1"/>
     <col min="8" max="8" width="50.08984375" customWidth="1"/>
+    <col min="10" max="10" width="7" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="2.54296875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
@@ -733,10 +736,10 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
@@ -744,29 +747,29 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="F2" s="16" t="s">
         <v>12</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>13</v>
       </c>
       <c r="G2" s="17">
         <f t="shared" ref="G2:G15" si="0">IF(AND(E2="Alta",F2="Alto"),$K$3*$K$3,IF(AND(E2="Alta",F2="Medio"),$K$3*$K$4,IF(AND(E2="Alta",F2="Bajo"),$K$3*$K$5,IF(AND(E2="Media",F2="Alto"),$K$4*$K$3,IF(AND(E2="Media",F2="Medio"),$K$4*$K$4,IF(AND(E2="Media",F2="Bajo"),$K$4*$K$5,IF(AND(E2="Baja",F2="Alto"),$K$5*$K$3,IF(AND(E2="Baja",F2="Medio"),$K$5*$K$4,IF(AND(E2="Baja",F2="Bajo"),$K$5*$K$5,0)))))))))</f>
         <v>9</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="18" t="s">
         <v>14</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
@@ -774,31 +777,31 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="E3" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>12</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>13</v>
       </c>
       <c r="G3" s="17">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="3">
+        <v>18</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="18">
         <v>3</v>
       </c>
     </row>
@@ -807,31 +810,31 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E4" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="16" t="s">
         <v>12</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>13</v>
       </c>
       <c r="G4" s="17">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="H4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="3">
+      <c r="K4" s="18">
         <v>2</v>
       </c>
     </row>
@@ -840,31 +843,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="F5" s="16" t="s">
         <v>28</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>29</v>
       </c>
       <c r="G5" s="17">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5" s="3">
+        <v>29</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="18">
         <v>1</v>
       </c>
     </row>
@@ -873,26 +876,26 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="16" t="s">
         <v>33</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>34</v>
       </c>
       <c r="G6" s="17">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="25" x14ac:dyDescent="0.25">
@@ -900,26 +903,26 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="E7" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" s="17">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
@@ -927,26 +930,26 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="E8" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G8" s="17">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
@@ -954,26 +957,26 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="E9" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G9" s="17">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="25" x14ac:dyDescent="0.25">
@@ -981,26 +984,26 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="E10" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="16" t="s">
         <v>28</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>29</v>
       </c>
       <c r="G10" s="17">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="25" x14ac:dyDescent="0.25">
@@ -1008,26 +1011,26 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>54</v>
-      </c>
       <c r="E11" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G11" s="17">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
@@ -1035,26 +1038,26 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="E12" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G12" s="17">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
@@ -1062,26 +1065,26 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="E13" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G13" s="17">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
@@ -1089,26 +1092,26 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>66</v>
-      </c>
       <c r="E14" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G14" s="17">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
@@ -1116,26 +1119,26 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="E15" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G15" s="17">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1412,6 +1415,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1438,7 +1442,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>4</v>
@@ -1449,19 +1453,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1469,16 +1473,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="8">
         <v>5</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G4" s="7"/>
     </row>
@@ -1487,14 +1491,14 @@
         <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G5" s="6">
         <v>12</v>
@@ -1505,19 +1509,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1525,7 +1529,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1533,7 +1537,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1541,7 +1545,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1549,7 +1553,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1557,7 +1561,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1565,7 +1569,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1573,7 +1577,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1581,7 +1585,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1589,7 +1593,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1597,7 +1601,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>